<commit_message>
[fix] path missing & main scene inventory
</commit_message>
<xml_diff>
--- a/SpartaFarming/Util/excel_files/CropGrowingInfo.xlsx
+++ b/SpartaFarming/Util/excel_files/CropGrowingInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anbak\SpartaFarming\SpartaFarming\Util\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087CD0EB-14EC-4843-A18E-F5CC3D34B3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E23F263-E0E1-458C-B229-D2F09AF4E399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="1950" windowWidth="19470" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15585" yWindow="4545" windowWidth="19470" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,10 +464,16 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="5" max="5" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="14.375" customWidth="1"/>
+    <col min="8" max="8" width="12.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -600,13 +606,13 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -615,10 +621,10 @@
         <v>2</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>